<commit_message>
(v2.1.1.9051) fix VGS mo code
</commit_message>
<xml_diff>
--- a/data-raw/microorganisms.codes.xlsx
+++ b/data-raw/microorganisms.codes.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7229" uniqueCount="7229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7227" uniqueCount="7227">
   <si>
     <t xml:space="preserve">code</t>
   </si>
@@ -21255,12 +21255,6 @@
   </si>
   <si>
     <t xml:space="preserve">VGC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B_VGCCC_SLMN</t>
   </si>
   <si>
     <t xml:space="preserve">VHI</t>
@@ -60915,15 +60909,15 @@
         <v>7081</v>
       </c>
       <c r="B4861" t="s">
-        <v>7082</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4862">
       <c r="A4862" t="s">
+        <v>7082</v>
+      </c>
+      <c r="B4862" t="s">
         <v>7083</v>
-      </c>
-      <c r="B4862" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4863">
@@ -60931,15 +60925,15 @@
         <v>7084</v>
       </c>
       <c r="B4863" t="s">
-        <v>7085</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4864">
       <c r="A4864" t="s">
+        <v>7085</v>
+      </c>
+      <c r="B4864" t="s">
         <v>7086</v>
-      </c>
-      <c r="B4864" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="4865">
@@ -60947,23 +60941,23 @@
         <v>7087</v>
       </c>
       <c r="B4865" t="s">
-        <v>7088</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4866">
       <c r="A4866" t="s">
-        <v>7089</v>
+        <v>7088</v>
       </c>
       <c r="B4866" t="s">
-        <v>295</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4867">
       <c r="A4867" t="s">
+        <v>7089</v>
+      </c>
+      <c r="B4867" t="s">
         <v>7090</v>
-      </c>
-      <c r="B4867" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="4868">
@@ -60971,23 +60965,23 @@
         <v>7091</v>
       </c>
       <c r="B4868" t="s">
-        <v>7092</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4869">
       <c r="A4869" t="s">
-        <v>7093</v>
+        <v>7092</v>
       </c>
       <c r="B4869" t="s">
-        <v>121</v>
+        <v>7066</v>
       </c>
     </row>
     <row r="4870">
       <c r="A4870" t="s">
+        <v>7093</v>
+      </c>
+      <c r="B4870" t="s">
         <v>7094</v>
-      </c>
-      <c r="B4870" t="s">
-        <v>7066</v>
       </c>
     </row>
     <row r="4871">
@@ -60995,23 +60989,23 @@
         <v>7095</v>
       </c>
       <c r="B4871" t="s">
-        <v>7096</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4872">
       <c r="A4872" t="s">
-        <v>7097</v>
+        <v>7096</v>
       </c>
       <c r="B4872" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4873">
       <c r="A4873" t="s">
+        <v>7097</v>
+      </c>
+      <c r="B4873" t="s">
         <v>7098</v>
-      </c>
-      <c r="B4873" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="4874">
@@ -61027,15 +61021,15 @@
         <v>7101</v>
       </c>
       <c r="B4875" t="s">
-        <v>7102</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4876">
       <c r="A4876" t="s">
+        <v>7102</v>
+      </c>
+      <c r="B4876" t="s">
         <v>7103</v>
-      </c>
-      <c r="B4876" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="4877">
@@ -61043,39 +61037,39 @@
         <v>7104</v>
       </c>
       <c r="B4877" t="s">
-        <v>7105</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4878">
       <c r="A4878" t="s">
-        <v>7106</v>
+        <v>7105</v>
       </c>
       <c r="B4878" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4879">
       <c r="A4879" t="s">
-        <v>7107</v>
+        <v>7106</v>
       </c>
       <c r="B4879" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4880">
       <c r="A4880" t="s">
-        <v>7108</v>
+        <v>7107</v>
       </c>
       <c r="B4880" t="s">
-        <v>306</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4881">
       <c r="A4881" t="s">
+        <v>7108</v>
+      </c>
+      <c r="B4881" t="s">
         <v>7109</v>
-      </c>
-      <c r="B4881" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4882">
@@ -61083,60 +61077,60 @@
         <v>7110</v>
       </c>
       <c r="B4882" t="s">
-        <v>7111</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4883">
       <c r="A4883" t="s">
-        <v>7112</v>
+        <v>7111</v>
       </c>
       <c r="B4883" t="s">
-        <v>121</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4884">
       <c r="A4884" t="s">
-        <v>7113</v>
+        <v>7112</v>
       </c>
       <c r="B4884" t="s">
-        <v>300</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4885">
       <c r="A4885" t="s">
-        <v>7114</v>
+        <v>7113</v>
       </c>
       <c r="B4885" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4886">
       <c r="A4886" t="s">
-        <v>7115</v>
+        <v>7114</v>
       </c>
       <c r="B4886" t="s">
-        <v>38</v>
+        <v>7100</v>
       </c>
     </row>
     <row r="4887">
       <c r="A4887" t="s">
-        <v>7116</v>
+        <v>7115</v>
       </c>
       <c r="B4887" t="s">
-        <v>7102</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4888">
       <c r="A4888" t="s">
-        <v>7117</v>
+        <v>7116</v>
       </c>
       <c r="B4888" t="s">
-        <v>304</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4889">
       <c r="A4889" t="s">
-        <v>7118</v>
+        <v>7117</v>
       </c>
       <c r="B4889" t="s">
         <v>121</v>
@@ -61144,58 +61138,58 @@
     </row>
     <row r="4890">
       <c r="A4890" t="s">
-        <v>7119</v>
+        <v>7118</v>
       </c>
       <c r="B4890" t="s">
-        <v>121</v>
+        <v>580</v>
       </c>
     </row>
     <row r="4891">
       <c r="A4891" t="s">
-        <v>7120</v>
+        <v>7119</v>
       </c>
       <c r="B4891" t="s">
-        <v>580</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4892">
       <c r="A4892" t="s">
-        <v>7121</v>
+        <v>7120</v>
       </c>
       <c r="B4892" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4893">
       <c r="A4893" t="s">
-        <v>7122</v>
+        <v>7121</v>
       </c>
       <c r="B4893" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4894">
       <c r="A4894" t="s">
-        <v>7123</v>
+        <v>7122</v>
       </c>
       <c r="B4894" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4895">
       <c r="A4895" t="s">
-        <v>7124</v>
+        <v>7123</v>
       </c>
       <c r="B4895" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4896">
       <c r="A4896" t="s">
+        <v>7124</v>
+      </c>
+      <c r="B4896" t="s">
         <v>7125</v>
-      </c>
-      <c r="B4896" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4897">
@@ -61203,31 +61197,31 @@
         <v>7126</v>
       </c>
       <c r="B4897" t="s">
-        <v>7127</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4898">
       <c r="A4898" t="s">
-        <v>7128</v>
+        <v>7127</v>
       </c>
       <c r="B4898" t="s">
-        <v>15</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4899">
       <c r="A4899" t="s">
-        <v>7129</v>
+        <v>7128</v>
       </c>
       <c r="B4899" t="s">
-        <v>306</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4900">
       <c r="A4900" t="s">
+        <v>7129</v>
+      </c>
+      <c r="B4900" t="s">
         <v>7130</v>
-      </c>
-      <c r="B4900" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4901">
@@ -61243,31 +61237,31 @@
         <v>7133</v>
       </c>
       <c r="B4902" t="s">
-        <v>7134</v>
+        <v>7130</v>
       </c>
     </row>
     <row r="4903">
       <c r="A4903" t="s">
-        <v>7135</v>
+        <v>7134</v>
       </c>
       <c r="B4903" t="s">
-        <v>7132</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="4904">
       <c r="A4904" t="s">
-        <v>7136</v>
+        <v>7135</v>
       </c>
       <c r="B4904" t="s">
-        <v>2916</v>
+        <v>7132</v>
       </c>
     </row>
     <row r="4905">
       <c r="A4905" t="s">
+        <v>7136</v>
+      </c>
+      <c r="B4905" t="s">
         <v>7137</v>
-      </c>
-      <c r="B4905" t="s">
-        <v>7134</v>
       </c>
     </row>
     <row r="4906">
@@ -61275,15 +61269,15 @@
         <v>7138</v>
       </c>
       <c r="B4906" t="s">
-        <v>7139</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="4907">
       <c r="A4907" t="s">
+        <v>7139</v>
+      </c>
+      <c r="B4907" t="s">
         <v>7140</v>
-      </c>
-      <c r="B4907" t="s">
-        <v>2916</v>
       </c>
     </row>
     <row r="4908">
@@ -61299,20 +61293,20 @@
         <v>7143</v>
       </c>
       <c r="B4909" t="s">
-        <v>7144</v>
+        <v>3447</v>
       </c>
     </row>
     <row r="4910">
       <c r="A4910" t="s">
-        <v>7145</v>
+        <v>7144</v>
       </c>
       <c r="B4910" t="s">
-        <v>3447</v>
+        <v>962</v>
       </c>
     </row>
     <row r="4911">
       <c r="A4911" t="s">
-        <v>7146</v>
+        <v>7145</v>
       </c>
       <c r="B4911" t="s">
         <v>962</v>
@@ -61320,10 +61314,10 @@
     </row>
     <row r="4912">
       <c r="A4912" t="s">
+        <v>7146</v>
+      </c>
+      <c r="B4912" t="s">
         <v>7147</v>
-      </c>
-      <c r="B4912" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="4913">
@@ -61339,12 +61333,12 @@
         <v>7150</v>
       </c>
       <c r="B4914" t="s">
-        <v>7151</v>
+        <v>964</v>
       </c>
     </row>
     <row r="4915">
       <c r="A4915" t="s">
-        <v>7152</v>
+        <v>7151</v>
       </c>
       <c r="B4915" t="s">
         <v>964</v>
@@ -61352,31 +61346,31 @@
     </row>
     <row r="4916">
       <c r="A4916" t="s">
-        <v>7153</v>
+        <v>7152</v>
       </c>
       <c r="B4916" t="s">
-        <v>964</v>
+        <v>7142</v>
       </c>
     </row>
     <row r="4917">
       <c r="A4917" t="s">
-        <v>7154</v>
+        <v>7153</v>
       </c>
       <c r="B4917" t="s">
-        <v>7144</v>
+        <v>964</v>
       </c>
     </row>
     <row r="4918">
       <c r="A4918" t="s">
-        <v>7155</v>
+        <v>7154</v>
       </c>
       <c r="B4918" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
     </row>
     <row r="4919">
       <c r="A4919" t="s">
-        <v>7156</v>
+        <v>7155</v>
       </c>
       <c r="B4919" t="s">
         <v>966</v>
@@ -61384,10 +61378,10 @@
     </row>
     <row r="4920">
       <c r="A4920" t="s">
+        <v>7156</v>
+      </c>
+      <c r="B4920" t="s">
         <v>7157</v>
-      </c>
-      <c r="B4920" t="s">
-        <v>966</v>
       </c>
     </row>
     <row r="4921">
@@ -61395,15 +61389,15 @@
         <v>7158</v>
       </c>
       <c r="B4921" t="s">
-        <v>7159</v>
+        <v>7157</v>
       </c>
     </row>
     <row r="4922">
       <c r="A4922" t="s">
+        <v>7159</v>
+      </c>
+      <c r="B4922" t="s">
         <v>7160</v>
-      </c>
-      <c r="B4922" t="s">
-        <v>7159</v>
       </c>
     </row>
     <row r="4923">
@@ -61411,47 +61405,47 @@
         <v>7161</v>
       </c>
       <c r="B4923" t="s">
-        <v>7162</v>
+        <v>7140</v>
       </c>
     </row>
     <row r="4924">
       <c r="A4924" t="s">
-        <v>7163</v>
+        <v>7162</v>
       </c>
       <c r="B4924" t="s">
-        <v>7142</v>
+        <v>7160</v>
       </c>
     </row>
     <row r="4925">
       <c r="A4925" t="s">
-        <v>7164</v>
+        <v>7163</v>
       </c>
       <c r="B4925" t="s">
-        <v>7162</v>
+        <v>7147</v>
       </c>
     </row>
     <row r="4926">
       <c r="A4926" t="s">
-        <v>7165</v>
+        <v>7164</v>
       </c>
       <c r="B4926" t="s">
-        <v>7149</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="4927">
       <c r="A4927" t="s">
-        <v>7166</v>
+        <v>7165</v>
       </c>
       <c r="B4927" t="s">
-        <v>1787</v>
+        <v>422</v>
       </c>
     </row>
     <row r="4928">
       <c r="A4928" t="s">
+        <v>7166</v>
+      </c>
+      <c r="B4928" t="s">
         <v>7167</v>
-      </c>
-      <c r="B4928" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="4929">
@@ -61459,15 +61453,15 @@
         <v>7168</v>
       </c>
       <c r="B4929" t="s">
-        <v>7169</v>
+        <v>424</v>
       </c>
     </row>
     <row r="4930">
       <c r="A4930" t="s">
+        <v>7169</v>
+      </c>
+      <c r="B4930" t="s">
         <v>7170</v>
-      </c>
-      <c r="B4930" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="4931">
@@ -61475,15 +61469,15 @@
         <v>7171</v>
       </c>
       <c r="B4931" t="s">
-        <v>7172</v>
+        <v>422</v>
       </c>
     </row>
     <row r="4932">
       <c r="A4932" t="s">
+        <v>7172</v>
+      </c>
+      <c r="B4932" t="s">
         <v>7173</v>
-      </c>
-      <c r="B4932" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="4933">
@@ -61507,15 +61501,15 @@
         <v>7178</v>
       </c>
       <c r="B4935" t="s">
-        <v>7179</v>
+        <v>7175</v>
       </c>
     </row>
     <row r="4936">
       <c r="A4936" t="s">
+        <v>7179</v>
+      </c>
+      <c r="B4936" t="s">
         <v>7180</v>
-      </c>
-      <c r="B4936" t="s">
-        <v>7177</v>
       </c>
     </row>
     <row r="4937">
@@ -61523,20 +61517,20 @@
         <v>7181</v>
       </c>
       <c r="B4937" t="s">
-        <v>7182</v>
+        <v>7180</v>
       </c>
     </row>
     <row r="4938">
       <c r="A4938" t="s">
-        <v>7183</v>
+        <v>7182</v>
       </c>
       <c r="B4938" t="s">
-        <v>7182</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4939">
       <c r="A4939" t="s">
-        <v>7184</v>
+        <v>7183</v>
       </c>
       <c r="B4939" t="s">
         <v>233</v>
@@ -61544,10 +61538,10 @@
     </row>
     <row r="4940">
       <c r="A4940" t="s">
+        <v>7184</v>
+      </c>
+      <c r="B4940" t="s">
         <v>7185</v>
-      </c>
-      <c r="B4940" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="4941">
@@ -61563,36 +61557,36 @@
         <v>7188</v>
       </c>
       <c r="B4942" t="s">
-        <v>7189</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4943">
       <c r="A4943" t="s">
-        <v>7190</v>
+        <v>7189</v>
       </c>
       <c r="B4943" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4944">
       <c r="A4944" t="s">
-        <v>7191</v>
+        <v>7190</v>
       </c>
       <c r="B4944" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4945">
       <c r="A4945" t="s">
-        <v>7192</v>
+        <v>7191</v>
       </c>
       <c r="B4945" t="s">
-        <v>226</v>
+        <v>7185</v>
       </c>
     </row>
     <row r="4946">
       <c r="A4946" t="s">
-        <v>7193</v>
+        <v>7192</v>
       </c>
       <c r="B4946" t="s">
         <v>7187</v>
@@ -61600,18 +61594,18 @@
     </row>
     <row r="4947">
       <c r="A4947" t="s">
-        <v>7194</v>
+        <v>7193</v>
       </c>
       <c r="B4947" t="s">
-        <v>7189</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4948">
       <c r="A4948" t="s">
+        <v>7194</v>
+      </c>
+      <c r="B4948" t="s">
         <v>7195</v>
-      </c>
-      <c r="B4948" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="4949">
@@ -61643,15 +61637,15 @@
         <v>7202</v>
       </c>
       <c r="B4952" t="s">
-        <v>7203</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4953">
       <c r="A4953" t="s">
+        <v>7203</v>
+      </c>
+      <c r="B4953" t="s">
         <v>7204</v>
-      </c>
-      <c r="B4953" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="4954">
@@ -61675,28 +61669,28 @@
         <v>7209</v>
       </c>
       <c r="B4956" t="s">
-        <v>7210</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4957">
       <c r="A4957" t="s">
-        <v>7211</v>
+        <v>7210</v>
       </c>
       <c r="B4957" t="s">
-        <v>226</v>
+        <v>7204</v>
       </c>
     </row>
     <row r="4958">
       <c r="A4958" t="s">
-        <v>7212</v>
+        <v>7211</v>
       </c>
       <c r="B4958" t="s">
-        <v>7206</v>
+        <v>7195</v>
       </c>
     </row>
     <row r="4959">
       <c r="A4959" t="s">
-        <v>7213</v>
+        <v>7212</v>
       </c>
       <c r="B4959" t="s">
         <v>7197</v>
@@ -61704,7 +61698,7 @@
     </row>
     <row r="4960">
       <c r="A4960" t="s">
-        <v>7214</v>
+        <v>7213</v>
       </c>
       <c r="B4960" t="s">
         <v>7199</v>
@@ -61712,7 +61706,7 @@
     </row>
     <row r="4961">
       <c r="A4961" t="s">
-        <v>7215</v>
+        <v>7214</v>
       </c>
       <c r="B4961" t="s">
         <v>7201</v>
@@ -61720,47 +61714,47 @@
     </row>
     <row r="4962">
       <c r="A4962" t="s">
-        <v>7216</v>
+        <v>7215</v>
       </c>
       <c r="B4962" t="s">
-        <v>7203</v>
+        <v>968</v>
       </c>
     </row>
     <row r="4963">
       <c r="A4963" t="s">
-        <v>7217</v>
+        <v>7216</v>
       </c>
       <c r="B4963" t="s">
-        <v>968</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="4964">
       <c r="A4964" t="s">
-        <v>7218</v>
+        <v>7217</v>
       </c>
       <c r="B4964" t="s">
-        <v>4094</v>
+        <v>968</v>
       </c>
     </row>
     <row r="4965">
       <c r="A4965" t="s">
-        <v>7219</v>
+        <v>7218</v>
       </c>
       <c r="B4965" t="s">
-        <v>968</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="4966">
       <c r="A4966" t="s">
-        <v>7220</v>
+        <v>7219</v>
       </c>
       <c r="B4966" t="s">
-        <v>4094</v>
+        <v>7206</v>
       </c>
     </row>
     <row r="4967">
       <c r="A4967" t="s">
-        <v>7221</v>
+        <v>7220</v>
       </c>
       <c r="B4967" t="s">
         <v>7208</v>
@@ -61768,26 +61762,26 @@
     </row>
     <row r="4968">
       <c r="A4968" t="s">
-        <v>7222</v>
+        <v>7221</v>
       </c>
       <c r="B4968" t="s">
-        <v>7210</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="4969">
       <c r="A4969" t="s">
-        <v>7223</v>
+        <v>7222</v>
       </c>
       <c r="B4969" t="s">
-        <v>2153</v>
+        <v>4618</v>
       </c>
     </row>
     <row r="4970">
       <c r="A4970" t="s">
+        <v>7223</v>
+      </c>
+      <c r="B4970" t="s">
         <v>7224</v>
-      </c>
-      <c r="B4970" t="s">
-        <v>4618</v>
       </c>
     </row>
     <row r="4971">
@@ -61795,22 +61789,14 @@
         <v>7225</v>
       </c>
       <c r="B4971" t="s">
-        <v>7226</v>
+        <v>5690</v>
       </c>
     </row>
     <row r="4972">
       <c r="A4972" t="s">
-        <v>7227</v>
+        <v>7226</v>
       </c>
       <c r="B4972" t="s">
-        <v>5690</v>
-      </c>
-    </row>
-    <row r="4973">
-      <c r="A4973" t="s">
-        <v>7228</v>
-      </c>
-      <c r="B4973" t="s">
         <v>5690</v>
       </c>
     </row>

</xml_diff>

<commit_message>
(v2.1.1.9081) HUGE microorganisms update for fungi!
</commit_message>
<xml_diff>
--- a/data-raw/microorganisms.codes.xlsx
+++ b/data-raw/microorganisms.codes.xlsx
@@ -4499,7 +4499,7 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>F_CANDD_KRUS</t>
+          <t>F_PICHI_KDRV</t>
         </is>
       </c>
     </row>
@@ -5123,7 +5123,7 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>F_BLSTM</t>
+          <t>F_CSPRM</t>
         </is>
       </c>
     </row>
@@ -5555,7 +5555,7 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>P_TXPL</t>
+          <t>C_TXPL</t>
         </is>
       </c>
     </row>
@@ -5567,7 +5567,7 @@
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>P_TXPL_GOND</t>
+          <t>C_TXPL_GOND</t>
         </is>
       </c>
     </row>
@@ -12575,7 +12575,7 @@
       </c>
       <c r="B1017" t="inlineStr">
         <is>
-          <t>F_CRVLR_ASTR</t>
+          <t>F_BPLRS_ASTR</t>
         </is>
       </c>
     </row>
@@ -13595,7 +13595,7 @@
       </c>
       <c r="B1102" t="inlineStr">
         <is>
-          <t>F_BLSTC_HMNS</t>
+          <t>C_BLSTC_HMNS</t>
         </is>
       </c>
     </row>
@@ -13823,7 +13823,7 @@
       </c>
       <c r="B1121" t="inlineStr">
         <is>
-          <t>F_BLSTM</t>
+          <t>F_CSPRM</t>
         </is>
       </c>
     </row>
@@ -13835,7 +13835,7 @@
       </c>
       <c r="B1122" t="inlineStr">
         <is>
-          <t>F_BLSTC_HMNS</t>
+          <t>C_BLSTC_HMNS</t>
         </is>
       </c>
     </row>
@@ -13847,7 +13847,7 @@
       </c>
       <c r="B1123" t="inlineStr">
         <is>
-          <t>F_BLSTC</t>
+          <t>C_BLSTC</t>
         </is>
       </c>
     </row>
@@ -13907,7 +13907,7 @@
       </c>
       <c r="B1128" t="inlineStr">
         <is>
-          <t>F_BLSTC</t>
+          <t>C_BLSTC</t>
         </is>
       </c>
     </row>
@@ -15083,7 +15083,7 @@
       </c>
       <c r="B1226" t="inlineStr">
         <is>
-          <t>F_CRVLR_SPCF</t>
+          <t>F_BPLRS_SPCF</t>
         </is>
       </c>
     </row>
@@ -16487,7 +16487,7 @@
       </c>
       <c r="B1343" t="inlineStr">
         <is>
-          <t>F_CANDD_GLLR</t>
+          <t>F_MYRZY_GLLR</t>
         </is>
       </c>
     </row>
@@ -16535,7 +16535,7 @@
       </c>
       <c r="B1347" t="inlineStr">
         <is>
-          <t>F_CANDD_KRUS</t>
+          <t>F_PICHI_KDRV</t>
         </is>
       </c>
     </row>
@@ -16559,7 +16559,7 @@
       </c>
       <c r="B1349" t="inlineStr">
         <is>
-          <t>F_CANDD_LMBC</t>
+          <t>F_PICHI_FRMN</t>
         </is>
       </c>
     </row>
@@ -17027,7 +17027,7 @@
       </c>
       <c r="B1388" t="inlineStr">
         <is>
-          <t>B_ANRCL_LRCM</t>
+          <t>B_ANRCL_AMNV</t>
         </is>
       </c>
     </row>
@@ -17915,7 +17915,7 @@
       </c>
       <c r="B1462" t="inlineStr">
         <is>
-          <t>F_CANDD_AFRC</t>
+          <t>F_CANDD_ALBC</t>
         </is>
       </c>
     </row>
@@ -17999,7 +17999,7 @@
       </c>
       <c r="B1469" t="inlineStr">
         <is>
-          <t>B_PNCLS_GHONI</t>
+          <t>B_PRCLS_GHON</t>
         </is>
       </c>
     </row>
@@ -19007,7 +19007,7 @@
       </c>
       <c r="B1553" t="inlineStr">
         <is>
-          <t>B_HTHWY_HSTLY</t>
+          <t>B_HTHWY_HSTL</t>
         </is>
       </c>
     </row>
@@ -19607,7 +19607,7 @@
       </c>
       <c r="B1603" t="inlineStr">
         <is>
-          <t>F_CANDD_KRUS</t>
+          <t>F_PICHI_KDRV</t>
         </is>
       </c>
     </row>
@@ -19787,7 +19787,7 @@
       </c>
       <c r="B1618" t="inlineStr">
         <is>
-          <t>F_CANDD_LMBC</t>
+          <t>F_PICHI_FRMN</t>
         </is>
       </c>
     </row>
@@ -21539,7 +21539,7 @@
       </c>
       <c r="B1764" t="inlineStr">
         <is>
-          <t>B_FCLCT_RTCM</t>
+          <t>B_FCLCT_ORTC</t>
         </is>
       </c>
     </row>
@@ -24107,7 +24107,7 @@
       </c>
       <c r="B1978" t="inlineStr">
         <is>
-          <t>B_LLLTT_NGNS</t>
+          <t>B_LLLTT_AMNG</t>
         </is>
       </c>
     </row>
@@ -24335,7 +24335,7 @@
       </c>
       <c r="B1997" t="inlineStr">
         <is>
-          <t>B_FCLCT_TRTM</t>
+          <t>B_FCLCT_CNTR</t>
         </is>
       </c>
     </row>
@@ -25055,7 +25055,7 @@
       </c>
       <c r="B2057" t="inlineStr">
         <is>
-          <t>B_ELZBT_PTCM</t>
+          <t>B_ELZBT_MNNG</t>
         </is>
       </c>
     </row>
@@ -26363,7 +26363,7 @@
       </c>
       <c r="B2166" t="inlineStr">
         <is>
-          <t>B_AGTHB_RECTL</t>
+          <t>B_AGTHB_RCTL</t>
         </is>
       </c>
     </row>
@@ -26447,7 +26447,7 @@
       </c>
       <c r="B2173" t="inlineStr">
         <is>
-          <t>B_ERWIN_ANNT</t>
+          <t>B_PANTO_ANNT</t>
         </is>
       </c>
     </row>
@@ -28943,7 +28943,7 @@
       </c>
       <c r="B2381" t="inlineStr">
         <is>
-          <t>F_FUSRM_PLLD</t>
+          <t>F_FUSRM_INCR</t>
         </is>
       </c>
     </row>
@@ -33143,7 +33143,7 @@
       </c>
       <c r="B2731" t="inlineStr">
         <is>
-          <t>B_KOCUR_ROSS</t>
+          <t>B_KOCUR_ROSE</t>
         </is>
       </c>
     </row>
@@ -33479,7 +33479,7 @@
       </c>
       <c r="B2759" t="inlineStr">
         <is>
-          <t>B_LCTBC_CTNFR</t>
+          <t>B_ERTHA_CTNF</t>
         </is>
       </c>
     </row>
@@ -34799,7 +34799,7 @@
       </c>
       <c r="B2869" t="inlineStr">
         <is>
-          <t>B_LLLTT_NGNS</t>
+          <t>B_LLLTT_AMNG</t>
         </is>
       </c>
     </row>
@@ -36695,7 +36695,7 @@
       </c>
       <c r="B3027" t="inlineStr">
         <is>
-          <t>F_MCRSP_DSTR</t>
+          <t>F_MCRSP_EQNM</t>
         </is>
       </c>
     </row>
@@ -37583,7 +37583,7 @@
       </c>
       <c r="B3101" t="inlineStr">
         <is>
-          <t>F_MCRSP_BLLR</t>
+          <t>F_MCRSP_FLVM</t>
         </is>
       </c>
     </row>
@@ -37607,7 +37607,7 @@
       </c>
       <c r="B3103" t="inlineStr">
         <is>
-          <t>F_MCRSP_DSTR</t>
+          <t>F_MCRSP_EQNM</t>
         </is>
       </c>
     </row>
@@ -37703,7 +37703,7 @@
       </c>
       <c r="B3111" t="inlineStr">
         <is>
-          <t>F_MCRSP_VNBR</t>
+          <t>F_MCRSP_GLLN</t>
         </is>
       </c>
     </row>
@@ -38375,7 +38375,7 @@
       </c>
       <c r="B3167" t="inlineStr">
         <is>
-          <t>B_MRXLL_TFRA</t>
+          <t>B_RMRLL_TFRA</t>
         </is>
       </c>
     </row>
@@ -39323,7 +39323,7 @@
       </c>
       <c r="B3246" t="inlineStr">
         <is>
-          <t>F_MCRSP_VNBR</t>
+          <t>F_MCRSP_GLLN</t>
         </is>
       </c>
     </row>
@@ -40595,7 +40595,7 @@
       </c>
       <c r="B3352" t="inlineStr">
         <is>
-          <t>B_MYRDS_DRTM</t>
+          <t>B_MYRDS_DRTS</t>
         </is>
       </c>
     </row>
@@ -40715,7 +40715,7 @@
       </c>
       <c r="B3362" t="inlineStr">
         <is>
-          <t>AN_NECTR_AMRC</t>
+          <t>F_NECATR_AMRC</t>
         </is>
       </c>
     </row>
@@ -40919,7 +40919,7 @@
       </c>
       <c r="B3379" t="inlineStr">
         <is>
-          <t>AN_NECTR_AMRC</t>
+          <t>F_NECATR_AMRC</t>
         </is>
       </c>
     </row>
@@ -44075,7 +44075,7 @@
       </c>
       <c r="B3642" t="inlineStr">
         <is>
-          <t>F_PICHI_FRNS</t>
+          <t>F_MLLRZ_FRNS</t>
         </is>
       </c>
     </row>
@@ -45215,7 +45215,7 @@
       </c>
       <c r="B3737" t="inlineStr">
         <is>
-          <t>B_RDNTB_PNMTR</t>
+          <t>B_RDNTB_PNMT</t>
         </is>
       </c>
     </row>
@@ -48023,7 +48023,7 @@
       </c>
       <c r="B3971" t="inlineStr">
         <is>
-          <t>F_RHZPS_ORYZ</t>
+          <t>F_RHZPS_ARRH</t>
         </is>
       </c>
     </row>
@@ -49907,7 +49907,7 @@
       </c>
       <c r="B4128" t="inlineStr">
         <is>
-          <t>F_SCLCB_CNST</t>
+          <t>F_OCHRC_CNST</t>
         </is>
       </c>
     </row>
@@ -51407,7 +51407,7 @@
       </c>
       <c r="B4253" t="inlineStr">
         <is>
-          <t>F_SCLCB_HMCL</t>
+          <t>F_OCHRC_HMCL</t>
         </is>
       </c>
     </row>
@@ -56363,7 +56363,7 @@
       </c>
       <c r="B4666" t="inlineStr">
         <is>
-          <t>F_TRCHP_EQNM</t>
+          <t>F_TRCHP_TNSR</t>
         </is>
       </c>
     </row>
@@ -56435,7 +56435,7 @@
       </c>
       <c r="B4672" t="inlineStr">
         <is>
-          <t>P_TXPL_GOND</t>
+          <t>C_TXPL_GOND</t>
         </is>
       </c>
     </row>
@@ -56519,7 +56519,7 @@
       </c>
       <c r="B4679" t="inlineStr">
         <is>
-          <t>B_CANDD_HMLN-C</t>
+          <t>F_CANDD_HMLN-C</t>
         </is>
       </c>
     </row>
@@ -56591,7 +56591,7 @@
       </c>
       <c r="B4685" t="inlineStr">
         <is>
-          <t>F_TRCHP_MGNN</t>
+          <t>F_TRCHP_RBRM</t>
         </is>
       </c>
     </row>
@@ -56663,7 +56663,7 @@
       </c>
       <c r="B4691" t="inlineStr">
         <is>
-          <t>P_TXPL</t>
+          <t>C_TXPL</t>
         </is>
       </c>
     </row>
@@ -56699,7 +56699,7 @@
       </c>
       <c r="B4694" t="inlineStr">
         <is>
-          <t>P_TXPL_GOND</t>
+          <t>C_TXPL_GOND</t>
         </is>
       </c>
     </row>
@@ -57215,7 +57215,7 @@
       </c>
       <c r="B4737" t="inlineStr">
         <is>
-          <t>F_TRCHP_EQNM</t>
+          <t>F_TRCHP_TNSR</t>
         </is>
       </c>
     </row>
@@ -57227,7 +57227,7 @@
       </c>
       <c r="B4738" t="inlineStr">
         <is>
-          <t>F_TRCHP_FSCH</t>
+          <t>F_TRCHP_RBRM</t>
         </is>
       </c>
     </row>
@@ -57251,7 +57251,7 @@
       </c>
       <c r="B4740" t="inlineStr">
         <is>
-          <t>F_TRCHP_FLVM</t>
+          <t>F_TRCHP_RBRM</t>
         </is>
       </c>
     </row>
@@ -57311,7 +57311,7 @@
       </c>
       <c r="B4745" t="inlineStr">
         <is>
-          <t>F_TRCHP_KANE</t>
+          <t>F_TRCHP_RBRM</t>
         </is>
       </c>
     </row>
@@ -57323,7 +57323,7 @@
       </c>
       <c r="B4746" t="inlineStr">
         <is>
-          <t>F_TRCHP_LNGF</t>
+          <t>F_ADRMA_FLVM</t>
         </is>
       </c>
     </row>
@@ -57335,7 +57335,7 @@
       </c>
       <c r="B4747" t="inlineStr">
         <is>
-          <t>F_TRCHP_MGNN</t>
+          <t>F_TRCHP_RBRM</t>
         </is>
       </c>
     </row>
@@ -57371,7 +57371,7 @@
       </c>
       <c r="B4750" t="inlineStr">
         <is>
-          <t>F_TRCHP_RBTS</t>
+          <t>F_TRCHP_RBRM</t>
         </is>
       </c>
     </row>
@@ -57419,7 +57419,7 @@
       </c>
       <c r="B4754" t="inlineStr">
         <is>
-          <t>F_TRCHP_SDNN</t>
+          <t>F_TRCHP_VLCM</t>
         </is>
       </c>
     </row>
@@ -57539,7 +57539,7 @@
       </c>
       <c r="B4764" t="inlineStr">
         <is>
-          <t>F_TRCHP_YAND</t>
+          <t>F_TRCHP_VLCM</t>
         </is>
       </c>
     </row>
@@ -57923,7 +57923,7 @@
       </c>
       <c r="B4796" t="inlineStr">
         <is>
-          <t>F_TRCHP_SDNN</t>
+          <t>F_TRCHP_VLCM</t>
         </is>
       </c>
     </row>

</xml_diff>